<commit_message>
remove previous excel script
</commit_message>
<xml_diff>
--- a/swertres/excel_results_4.xlsx
+++ b/swertres/excel_results_4.xlsx
@@ -72,11 +72,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="0066cc33"/>
       </patternFill>
     </fill>
@@ -93,6 +88,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0033ff33"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,7 +220,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -247,6 +247,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -254,9 +257,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
@@ -268,7 +268,7 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2464,7 +2464,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P11" s="17" t="inlineStr">
+      <c r="P11" s="9" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -4252,7 +4252,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK20" s="17" t="inlineStr">
+      <c r="AK20" s="16" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -7717,7 +7717,7 @@
           <t>05</t>
         </is>
       </c>
-      <c r="B40" s="5" t="inlineStr">
+      <c r="B40" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -8453,7 +8453,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK43" s="16" t="inlineStr">
+      <c r="AK43" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -8959,7 +8959,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="Z46" s="13" t="inlineStr">
+      <c r="Z46" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -9415,7 +9415,7 @@
           <t>545</t>
         </is>
       </c>
-      <c r="E49" s="17" t="inlineStr">
+      <c r="E49" s="6" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -11779,7 +11779,7 @@
           <t>146</t>
         </is>
       </c>
-      <c r="AC61" s="17" t="inlineStr">
+      <c r="AC61" s="14" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -12350,7 +12350,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE64" s="17" t="inlineStr">
+      <c r="AE64" s="14" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -12579,7 +12579,7 @@
           <t>31</t>
         </is>
       </c>
-      <c r="B66" s="17" t="inlineStr">
+      <c r="B66" s="5" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -13115,7 +13115,7 @@
           <t>054</t>
         </is>
       </c>
-      <c r="Q69" s="17" t="inlineStr">
+      <c r="Q69" s="10" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -14434,7 +14434,7 @@
           <t>373</t>
         </is>
       </c>
-      <c r="S76" s="17" t="inlineStr">
+      <c r="S76" s="10" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -15097,7 +15097,7 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B80" s="5" t="inlineStr">
+      <c r="B80" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -16082,7 +16082,7 @@
           <t>064</t>
         </is>
       </c>
-      <c r="L85" s="8" t="inlineStr">
+      <c r="L85" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -16374,7 +16374,7 @@
           <t>100</t>
         </is>
       </c>
-      <c r="AG86" s="15" t="inlineStr">
+      <c r="AG86" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -16556,7 +16556,7 @@
           <t>102</t>
         </is>
       </c>
-      <c r="AF87" s="17" t="inlineStr">
+      <c r="AF87" s="15" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -16668,7 +16668,7 @@
           <t>405</t>
         </is>
       </c>
-      <c r="Q88" s="17" t="inlineStr">
+      <c r="Q88" s="10" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -18588,7 +18588,7 @@
           <t>155</t>
         </is>
       </c>
-      <c r="AA98" s="13" t="inlineStr">
+      <c r="AA98" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -19271,7 +19271,7 @@
           <t>173</t>
         </is>
       </c>
-      <c r="AH102" s="15" t="inlineStr">
+      <c r="AH102" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -19560,7 +19560,7 @@
           <t>000</t>
         </is>
       </c>
-      <c r="Q104" s="10" t="inlineStr">
+      <c r="Q104" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -19787,7 +19787,7 @@
           <t>348</t>
         </is>
       </c>
-      <c r="Y105" s="17" t="inlineStr">
+      <c r="Y105" s="12" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -19859,7 +19859,7 @@
           <t>05</t>
         </is>
       </c>
-      <c r="B106" s="5" t="inlineStr">
+      <c r="B106" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -21380,7 +21380,7 @@
           <t>399</t>
         </is>
       </c>
-      <c r="G114" s="6" t="inlineStr">
+      <c r="G114" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -22310,7 +22310,7 @@
           <t>954</t>
         </is>
       </c>
-      <c r="F119" s="17" t="inlineStr">
+      <c r="F119" s="6" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -22477,7 +22477,7 @@
           <t>19</t>
         </is>
       </c>
-      <c r="B120" s="5" t="inlineStr">
+      <c r="B120" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -22552,7 +22552,7 @@
           <t>537</t>
         </is>
       </c>
-      <c r="Q120" s="10" t="inlineStr">
+      <c r="Q120" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -23375,7 +23375,7 @@
           <t>536</t>
         </is>
       </c>
-      <c r="AF124" s="17" t="inlineStr">
+      <c r="AF124" s="15" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -23901,7 +23901,7 @@
           <t>188</t>
         </is>
       </c>
-      <c r="Y127" s="12" t="inlineStr">
+      <c r="Y127" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -24143,7 +24143,7 @@
           <t>764</t>
         </is>
       </c>
-      <c r="AJ128" s="16" t="inlineStr">
+      <c r="AJ128" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -24185,7 +24185,7 @@
           <t>686</t>
         </is>
       </c>
-      <c r="G129" s="6" t="inlineStr">
+      <c r="G129" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -25347,7 +25347,7 @@
           <t>193</t>
         </is>
       </c>
-      <c r="AI135" s="16" t="inlineStr">
+      <c r="AI135" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -25581,7 +25581,7 @@
           <t>807</t>
         </is>
       </c>
-      <c r="G137" s="6" t="inlineStr">
+      <c r="G137" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -26910,7 +26910,7 @@
           <t>406</t>
         </is>
       </c>
-      <c r="K144" s="8" t="inlineStr">
+      <c r="K144" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -26950,7 +26950,7 @@
           <t>329</t>
         </is>
       </c>
-      <c r="S144" s="17" t="inlineStr">
+      <c r="S144" s="10" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -27531,7 +27531,7 @@
           <t>920</t>
         </is>
       </c>
-      <c r="W147" s="12" t="inlineStr">
+      <c r="W147" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -28007,7 +28007,7 @@
           <t>484</t>
         </is>
       </c>
-      <c r="F150" s="17" t="inlineStr">
+      <c r="F150" s="6" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -28229,7 +28229,7 @@
           <t>083</t>
         </is>
       </c>
-      <c r="M151" s="17" t="inlineStr">
+      <c r="M151" s="8" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -28401,7 +28401,7 @@
           <t>486</t>
         </is>
       </c>
-      <c r="J152" s="17" t="inlineStr">
+      <c r="J152" s="7" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -28521,7 +28521,7 @@
           <t>447</t>
         </is>
       </c>
-      <c r="AH152" s="15" t="inlineStr">
+      <c r="AH152" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -29194,7 +29194,7 @@
           <t>510</t>
         </is>
       </c>
-      <c r="S156" s="17" t="inlineStr">
+      <c r="S156" s="10" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -29239,7 +29239,7 @@
           <t>174</t>
         </is>
       </c>
-      <c r="AB156" s="13" t="inlineStr">
+      <c r="AB156" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -29254,7 +29254,7 @@
           <t>057</t>
         </is>
       </c>
-      <c r="AE156" s="17" t="inlineStr">
+      <c r="AE156" s="14" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -29416,7 +29416,7 @@
           <t>812</t>
         </is>
       </c>
-      <c r="Z157" s="17" t="inlineStr">
+      <c r="Z157" s="13" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -29830,7 +29830,7 @@
           <t>195</t>
         </is>
       </c>
-      <c r="AH159" s="15" t="inlineStr">
+      <c r="AH159" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -30184,7 +30184,7 @@
           <t>917</t>
         </is>
       </c>
-      <c r="AD161" s="14" t="inlineStr">
+      <c r="AD161" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -30563,7 +30563,7 @@
           <t>063</t>
         </is>
       </c>
-      <c r="AE163" s="14" t="inlineStr">
+      <c r="AE163" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -31505,7 +31505,7 @@
           <t>510</t>
         </is>
       </c>
-      <c r="O169" s="17" t="inlineStr">
+      <c r="O169" s="9" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -32243,7 +32243,7 @@
           <t>899</t>
         </is>
       </c>
-      <c r="M173" s="8" t="inlineStr">
+      <c r="M173" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -32632,7 +32632,7 @@
           <t>734</t>
         </is>
       </c>
-      <c r="P175" s="17" t="inlineStr">
+      <c r="P175" s="9" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -32924,7 +32924,7 @@
           <t>935</t>
         </is>
       </c>
-      <c r="AK176" s="17" t="inlineStr">
+      <c r="AK176" s="16" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -33315,7 +33315,7 @@
           <t>951</t>
         </is>
       </c>
-      <c r="C179" s="5" t="inlineStr">
+      <c r="C179" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -34143,7 +34143,7 @@
           <t>137</t>
         </is>
       </c>
-      <c r="S183" s="17" t="inlineStr">
+      <c r="S183" s="10" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -35098,7 +35098,7 @@
           <t>529</t>
         </is>
       </c>
-      <c r="W188" s="12" t="inlineStr">
+      <c r="W188" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -35245,7 +35245,7 @@
           <t>764</t>
         </is>
       </c>
-      <c r="O189" s="17" t="inlineStr">
+      <c r="O189" s="9" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -35447,7 +35447,7 @@
           <t>457</t>
         </is>
       </c>
-      <c r="R190" s="17" t="inlineStr">
+      <c r="R190" s="10" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -35472,7 +35472,7 @@
           <t>292</t>
         </is>
       </c>
-      <c r="W190" s="12" t="inlineStr">
+      <c r="W190" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -35953,7 +35953,7 @@
           <t>457</t>
         </is>
       </c>
-      <c r="G193" s="6" t="inlineStr">
+      <c r="G193" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -36437,7 +36437,7 @@
           <t>246</t>
         </is>
       </c>
-      <c r="AC195" s="17" t="inlineStr">
+      <c r="AC195" s="14" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -37868,7 +37868,7 @@
           <t>195</t>
         </is>
       </c>
-      <c r="AJ203" s="17" t="inlineStr">
+      <c r="AJ203" s="16" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -37920,7 +37920,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="I204" s="7" t="inlineStr">
+      <c r="I204" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -37990,7 +37990,7 @@
           <t>479</t>
         </is>
       </c>
-      <c r="W204" s="17" t="inlineStr">
+      <c r="W204" s="12" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -38925,7 +38925,7 @@
           <t>156</t>
         </is>
       </c>
-      <c r="W209" s="17" t="inlineStr">
+      <c r="W209" s="12" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -39042,7 +39042,7 @@
           <t>422</t>
         </is>
       </c>
-      <c r="I210" s="7" t="inlineStr">
+      <c r="I210" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -39072,7 +39072,7 @@
           <t>050</t>
         </is>
       </c>
-      <c r="O210" s="9" t="inlineStr">
+      <c r="O210" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -39224,7 +39224,7 @@
           <t>256</t>
         </is>
       </c>
-      <c r="H211" s="17" t="inlineStr">
+      <c r="H211" s="7" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -39688,7 +39688,7 @@
           <t>437</t>
         </is>
       </c>
-      <c r="Z213" s="17" t="inlineStr">
+      <c r="Z213" s="13" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -40219,7 +40219,7 @@
           <t>817</t>
         </is>
       </c>
-      <c r="T216" s="11" t="inlineStr">
+      <c r="T216" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -41089,7 +41089,7 @@
           <t>850</t>
         </is>
       </c>
-      <c r="G221" s="6" t="inlineStr">
+      <c r="G221" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -41376,7 +41376,7 @@
           <t>595</t>
         </is>
       </c>
-      <c r="AA222" s="13" t="inlineStr">
+      <c r="AA222" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -41401,7 +41401,7 @@
           <t>591</t>
         </is>
       </c>
-      <c r="AF222" s="15" t="inlineStr">
+      <c r="AF222" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -41645,7 +41645,7 @@
           <t>328</t>
         </is>
       </c>
-      <c r="F224" s="6" t="inlineStr">
+      <c r="F224" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -41655,7 +41655,7 @@
           <t>987</t>
         </is>
       </c>
-      <c r="H224" s="7" t="inlineStr">
+      <c r="H224" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -41952,7 +41952,7 @@
           <t>438</t>
         </is>
       </c>
-      <c r="AD225" s="14" t="inlineStr">
+      <c r="AD225" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -42321,7 +42321,7 @@
           <t>075</t>
         </is>
       </c>
-      <c r="AC227" s="17" t="inlineStr">
+      <c r="AC227" s="14" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -42361,7 +42361,7 @@
           <t>923</t>
         </is>
       </c>
-      <c r="AK227" s="16" t="inlineStr">
+      <c r="AK227" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -42585,7 +42585,7 @@
           <t>483</t>
         </is>
       </c>
-      <c r="G229" s="6" t="inlineStr">
+      <c r="G229" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -42792,7 +42792,7 @@
           <t>504</t>
         </is>
       </c>
-      <c r="K230" s="17" t="inlineStr">
+      <c r="K230" s="8" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -42944,7 +42944,7 @@
           <t>986</t>
         </is>
       </c>
-      <c r="D231" s="17" t="inlineStr">
+      <c r="D231" s="5" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -43560,7 +43560,7 @@
           <t>268</t>
         </is>
       </c>
-      <c r="AI234" s="17" t="inlineStr">
+      <c r="AI234" s="16" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -43914,7 +43914,7 @@
           <t>474</t>
         </is>
       </c>
-      <c r="AE236" s="14" t="inlineStr">
+      <c r="AE236" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -44001,7 +44001,7 @@
           <t>023</t>
         </is>
       </c>
-      <c r="K237" s="8" t="inlineStr">
+      <c r="K237" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -44016,7 +44016,7 @@
           <t>970</t>
         </is>
       </c>
-      <c r="N237" s="17" t="inlineStr">
+      <c r="N237" s="9" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -44607,7 +44607,7 @@
           <t>193</t>
         </is>
       </c>
-      <c r="T240" s="11" t="inlineStr">
+      <c r="T240" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -44921,12 +44921,12 @@
           <t>626</t>
         </is>
       </c>
-      <c r="H242" s="7" t="inlineStr">
+      <c r="H242" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
       </c>
-      <c r="I242" s="7" t="inlineStr">
+      <c r="I242" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -45552,7 +45552,7 @@
           <t>058</t>
         </is>
       </c>
-      <c r="V245" s="17" t="inlineStr">
+      <c r="V245" s="11" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -45709,7 +45709,7 @@
           <t>601</t>
         </is>
       </c>
-      <c r="P246" s="17" t="inlineStr">
+      <c r="P246" s="9" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -45996,7 +45996,7 @@
           <t>159</t>
         </is>
       </c>
-      <c r="AJ247" s="16" t="inlineStr">
+      <c r="AJ247" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -46402,7 +46402,7 @@
           <t>535</t>
         </is>
       </c>
-      <c r="E250" s="6" t="inlineStr">
+      <c r="E250" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -47180,7 +47180,7 @@
           <t>611</t>
         </is>
       </c>
-      <c r="K254" s="8" t="inlineStr">
+      <c r="K254" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -48115,7 +48115,7 @@
           <t>220</t>
         </is>
       </c>
-      <c r="K259" s="8" t="inlineStr">
+      <c r="K259" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -48240,7 +48240,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="AJ259" s="16" t="inlineStr">
+      <c r="AJ259" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -48272,7 +48272,7 @@
           <t>871</t>
         </is>
       </c>
-      <c r="E260" s="17" t="inlineStr">
+      <c r="E260" s="6" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -48454,7 +48454,7 @@
           <t>506</t>
         </is>
       </c>
-      <c r="D261" s="17" t="inlineStr">
+      <c r="D261" s="5" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -48883,7 +48883,7 @@
           <t>090</t>
         </is>
       </c>
-      <c r="O263" s="9" t="inlineStr">
+      <c r="O263" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -49506,7 +49506,7 @@
           <t>658</t>
         </is>
       </c>
-      <c r="J267" s="17" t="inlineStr">
+      <c r="J267" s="7" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -49950,7 +49950,7 @@
           <t>546</t>
         </is>
       </c>
-      <c r="X269" s="17" t="inlineStr">
+      <c r="X269" s="12" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -50658,7 +50658,7 @@
           <t>420</t>
         </is>
       </c>
-      <c r="P273" s="17" t="inlineStr">
+      <c r="P273" s="9" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -50790,7 +50790,7 @@
           <t>445</t>
         </is>
       </c>
-      <c r="E274" s="17" t="inlineStr">
+      <c r="E274" s="6" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -51578,7 +51578,7 @@
           <t>452</t>
         </is>
       </c>
-      <c r="M278" s="17" t="inlineStr">
+      <c r="M278" s="8" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -51638,7 +51638,7 @@
           <t>230</t>
         </is>
       </c>
-      <c r="Y278" s="12" t="inlineStr">
+      <c r="Y278" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -52047,7 +52047,7 @@
           <t>914</t>
         </is>
       </c>
-      <c r="AF280" s="17" t="inlineStr">
+      <c r="AF280" s="15" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -52244,7 +52244,7 @@
           <t>534</t>
         </is>
       </c>
-      <c r="AH281" s="15" t="inlineStr">
+      <c r="AH281" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -52548,7 +52548,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="T283" s="11" t="inlineStr">
+      <c r="T283" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -52790,7 +52790,7 @@
           <t>445</t>
         </is>
       </c>
-      <c r="AE284" s="17" t="inlineStr">
+      <c r="AE284" s="14" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -53211,7 +53211,7 @@
           <t>283</t>
         </is>
       </c>
-      <c r="C287" s="5" t="inlineStr">
+      <c r="C287" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -53650,7 +53650,7 @@
           <t>157</t>
         </is>
       </c>
-      <c r="P289" s="17" t="inlineStr">
+      <c r="P289" s="9" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -54104,7 +54104,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="AF291" s="17" t="inlineStr">
+      <c r="AF291" s="15" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -54373,7 +54373,7 @@
           <t>245</t>
         </is>
       </c>
-      <c r="K293" s="8" t="inlineStr">
+      <c r="K293" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -55054,7 +55054,7 @@
           <t>761</t>
         </is>
       </c>
-      <c r="AI296" s="17" t="inlineStr">
+      <c r="AI296" s="16" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -56158,7 +56158,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N303" s="9" t="inlineStr">
+      <c r="N303" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -56911,7 +56911,7 @@
           <t>048</t>
         </is>
       </c>
-      <c r="O307" s="17" t="inlineStr">
+      <c r="O307" s="9" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -57188,7 +57188,7 @@
           <t>772</t>
         </is>
       </c>
-      <c r="AG308" s="15" t="inlineStr">
+      <c r="AG308" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -58058,7 +58058,7 @@
           <t>249</t>
         </is>
       </c>
-      <c r="T313" s="17" t="inlineStr">
+      <c r="T313" s="11" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -58175,7 +58175,7 @@
           <t>037</t>
         </is>
       </c>
-      <c r="F314" s="17" t="inlineStr">
+      <c r="F314" s="6" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -58300,7 +58300,7 @@
           <t>363</t>
         </is>
       </c>
-      <c r="AE314" s="14" t="inlineStr">
+      <c r="AE314" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -58517,7 +58517,7 @@
           <t>882</t>
         </is>
       </c>
-      <c r="AK315" s="17" t="inlineStr">
+      <c r="AK315" s="16" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -59225,7 +59225,7 @@
           <t>156</t>
         </is>
       </c>
-      <c r="AC319" s="17" t="inlineStr">
+      <c r="AC319" s="14" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -59442,7 +59442,7 @@
           <t>217</t>
         </is>
       </c>
-      <c r="AI320" s="16" t="inlineStr">
+      <c r="AI320" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -59731,7 +59731,7 @@
           <t>018</t>
         </is>
       </c>
-      <c r="R322" s="10" t="inlineStr">
+      <c r="R322" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -60539,7 +60539,7 @@
           <t>820</t>
         </is>
       </c>
-      <c r="AD326" s="14" t="inlineStr">
+      <c r="AD326" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -61733,7 +61733,7 @@
           <t>977</t>
         </is>
       </c>
-      <c r="AA333" s="17" t="inlineStr">
+      <c r="AA333" s="13" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -62092,7 +62092,7 @@
           <t>805</t>
         </is>
       </c>
-      <c r="X335" s="12" t="inlineStr">
+      <c r="X335" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -62204,7 +62204,7 @@
           <t>747</t>
         </is>
       </c>
-      <c r="I336" s="7" t="inlineStr">
+      <c r="I336" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -62740,7 +62740,7 @@
           <t>341</t>
         </is>
       </c>
-      <c r="D339" s="17" t="inlineStr">
+      <c r="D339" s="5" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -62865,7 +62865,7 @@
           <t>657</t>
         </is>
       </c>
-      <c r="AC339" s="17" t="inlineStr">
+      <c r="AC339" s="14" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -63376,7 +63376,7 @@
           <t>832</t>
         </is>
       </c>
-      <c r="S342" s="17" t="inlineStr">
+      <c r="S342" s="10" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -63446,7 +63446,7 @@
           <t>913</t>
         </is>
       </c>
-      <c r="AG342" s="17" t="inlineStr">
+      <c r="AG342" s="15" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -64443,7 +64443,7 @@
           <t>582</t>
         </is>
       </c>
-      <c r="H348" s="7" t="inlineStr">
+      <c r="H348" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -65523,7 +65523,7 @@
           <t>791</t>
         </is>
       </c>
-      <c r="AK353" s="17" t="inlineStr">
+      <c r="AK353" s="16" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -65852,7 +65852,7 @@
           <t>926</t>
         </is>
       </c>
-      <c r="AB355" s="17" t="inlineStr">
+      <c r="AB355" s="13" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -65897,7 +65897,7 @@
           <t>547</t>
         </is>
       </c>
-      <c r="AK355" s="17" t="inlineStr">
+      <c r="AK355" s="16" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -66393,7 +66393,7 @@
           <t>867</t>
         </is>
       </c>
-      <c r="X358" s="12" t="inlineStr">
+      <c r="X358" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -68664,7 +68664,7 @@
           <t>621</t>
         </is>
       </c>
-      <c r="L371" s="8" t="inlineStr">
+      <c r="L371" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -68961,7 +68961,7 @@
           <t>972</t>
         </is>
       </c>
-      <c r="AH372" s="15" t="inlineStr">
+      <c r="AH372" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -70726,7 +70726,7 @@
           <t>691</t>
         </is>
       </c>
-      <c r="M382" s="8" t="inlineStr">
+      <c r="M382" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -70883,7 +70883,7 @@
           <t>765</t>
         </is>
       </c>
-      <c r="G383" s="17" t="inlineStr">
+      <c r="G383" s="6" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -71125,7 +71125,7 @@
           <t>854</t>
         </is>
       </c>
-      <c r="R384" s="10" t="inlineStr">
+      <c r="R384" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -71160,7 +71160,7 @@
           <t>198</t>
         </is>
       </c>
-      <c r="Y384" s="17" t="inlineStr">
+      <c r="Y384" s="12" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -71469,7 +71469,7 @@
           <t>043</t>
         </is>
       </c>
-      <c r="L386" s="17" t="inlineStr">
+      <c r="L386" s="8" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -71798,7 +71798,7 @@
           <t>675</t>
         </is>
       </c>
-      <c r="C388" s="17" t="inlineStr">
+      <c r="C388" s="5" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -72676,7 +72676,7 @@
           <t>975</t>
         </is>
       </c>
-      <c r="AC392" s="14" t="inlineStr">
+      <c r="AC392" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -72691,7 +72691,7 @@
           <t>864</t>
         </is>
       </c>
-      <c r="AF392" s="15" t="inlineStr">
+      <c r="AF392" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -72990,7 +72990,7 @@
           <t>868</t>
         </is>
       </c>
-      <c r="Q394" s="10" t="inlineStr">
+      <c r="Q394" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -73237,7 +73237,7 @@
           <t>733</t>
         </is>
       </c>
-      <c r="AC395" s="14" t="inlineStr">
+      <c r="AC395" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -73845,7 +73845,7 @@
           <t>011</t>
         </is>
       </c>
-      <c r="U399" s="11" t="inlineStr">
+      <c r="U399" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -74623,7 +74623,7 @@
           <t>360</t>
         </is>
       </c>
-      <c r="AA403" s="17" t="inlineStr">
+      <c r="AA403" s="13" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -75857,7 +75857,7 @@
           <t>299</t>
         </is>
       </c>
-      <c r="L410" s="17" t="inlineStr">
+      <c r="L410" s="8" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -76306,7 +76306,7 @@
           <t>019</t>
         </is>
       </c>
-      <c r="AA412" s="13" t="inlineStr">
+      <c r="AA412" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -76590,7 +76590,7 @@
           <t>683</t>
         </is>
       </c>
-      <c r="I414" s="17" t="inlineStr">
+      <c r="I414" s="7" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -76929,7 +76929,7 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B416" s="17" t="inlineStr">
+      <c r="B416" s="5" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -78248,7 +78248,7 @@
           <t>757</t>
         </is>
       </c>
-      <c r="D423" s="5" t="inlineStr">
+      <c r="D423" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -78560,7 +78560,7 @@
           <t>463</t>
         </is>
       </c>
-      <c r="AC424" s="17" t="inlineStr">
+      <c r="AC424" s="14" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -78697,7 +78697,7 @@
           <t>682</t>
         </is>
       </c>
-      <c r="S425" s="17" t="inlineStr">
+      <c r="S425" s="10" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -79861,7 +79861,7 @@
           <t>102</t>
         </is>
       </c>
-      <c r="J432" s="17" t="inlineStr">
+      <c r="J432" s="7" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -80265,12 +80265,12 @@
           <t>716</t>
         </is>
       </c>
-      <c r="P434" s="9" t="inlineStr">
+      <c r="P434" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
       </c>
-      <c r="Q434" s="17" t="inlineStr">
+      <c r="Q434" s="10" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -80704,7 +80704,7 @@
           <t>878</t>
         </is>
       </c>
-      <c r="AC436" s="14" t="inlineStr">
+      <c r="AC436" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -80761,7 +80761,7 @@
           <t>952</t>
         </is>
       </c>
-      <c r="C437" s="17" t="inlineStr">
+      <c r="C437" s="5" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -80926,7 +80926,7 @@
           <t>178</t>
         </is>
       </c>
-      <c r="AJ437" s="16" t="inlineStr">
+      <c r="AJ437" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -81539,7 +81539,7 @@
           <t>724</t>
         </is>
       </c>
-      <c r="I441" s="7" t="inlineStr">
+      <c r="I441" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -82008,7 +82008,7 @@
           <t>119</t>
         </is>
       </c>
-      <c r="AB443" s="17" t="inlineStr">
+      <c r="AB443" s="13" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -82033,7 +82033,7 @@
           <t>797</t>
         </is>
       </c>
-      <c r="AG443" s="15" t="inlineStr">
+      <c r="AG443" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -82085,7 +82085,7 @@
           <t>683</t>
         </is>
       </c>
-      <c r="F444" s="17" t="inlineStr">
+      <c r="F444" s="6" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -82676,7 +82676,7 @@
           <t>064</t>
         </is>
       </c>
-      <c r="L447" s="8" t="inlineStr">
+      <c r="L447" s="17" t="inlineStr">
         <is>
           <t>214</t>
         </is>
@@ -82686,7 +82686,7 @@
           <t>739</t>
         </is>
       </c>
-      <c r="N447" s="17" t="inlineStr">
+      <c r="N447" s="9" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -82726,7 +82726,7 @@
           <t>001</t>
         </is>
       </c>
-      <c r="V447" s="17" t="inlineStr">
+      <c r="V447" s="11" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -83464,7 +83464,7 @@
           <t>104</t>
         </is>
       </c>
-      <c r="T451" s="17" t="inlineStr">
+      <c r="T451" s="11" t="inlineStr">
         <is>
           <t>760</t>
         </is>
@@ -83833,12 +83833,12 @@
           <t>116</t>
         </is>
       </c>
-      <c r="S453" s="10" t="inlineStr">
+      <c r="S453" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
       </c>
-      <c r="T453" s="11" t="inlineStr">
+      <c r="T453" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -84045,7 +84045,7 @@
           <t>795</t>
         </is>
       </c>
-      <c r="X454" s="12" t="inlineStr">
+      <c r="X454" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -84439,7 +84439,7 @@
           <t>547</t>
         </is>
       </c>
-      <c r="AB456" s="13" t="inlineStr">
+      <c r="AB456" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>
@@ -84464,7 +84464,7 @@
           <t>612</t>
         </is>
       </c>
-      <c r="AG456" s="15" t="inlineStr">
+      <c r="AG456" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -84576,7 +84576,7 @@
           <t>807</t>
         </is>
       </c>
-      <c r="R457" s="17" t="inlineStr">
+      <c r="R457" s="10" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -84940,7 +84940,7 @@
           <t>139</t>
         </is>
       </c>
-      <c r="P459" s="17" t="inlineStr">
+      <c r="P459" s="9" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -86650,7 +86650,7 @@
           <t>973</t>
         </is>
       </c>
-      <c r="D469" s="17" t="inlineStr">
+      <c r="D469" s="5" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -87558,7 +87558,7 @@
           <t>665</t>
         </is>
       </c>
-      <c r="AJ473" s="16" t="inlineStr">
+      <c r="AJ473" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -87882,7 +87882,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Z475" s="13" t="inlineStr">
+      <c r="Z475" s="17" t="inlineStr">
         <is>
           <t>421</t>
         </is>
@@ -88448,7 +88448,7 @@
           <t>346</t>
         </is>
       </c>
-      <c r="AA478" s="13" t="inlineStr">
+      <c r="AA478" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -88914,7 +88914,7 @@
           <t>840</t>
         </is>
       </c>
-      <c r="H481" s="17" t="inlineStr">
+      <c r="H481" s="7" t="inlineStr">
         <is>
           <t>670</t>
         </is>
@@ -90490,7 +90490,7 @@
           <t>900</t>
         </is>
       </c>
-      <c r="X489" s="17" t="inlineStr">
+      <c r="X489" s="12" t="inlineStr">
         <is>
           <t>076</t>
         </is>
@@ -91829,7 +91829,7 @@
           <t>446</t>
         </is>
       </c>
-      <c r="F498" s="6" t="inlineStr">
+      <c r="F498" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -92495,7 +92495,7 @@
           <t>772</t>
         </is>
       </c>
-      <c r="H506" s="7" t="inlineStr">
+      <c r="H506" s="17" t="inlineStr">
         <is>
           <t>124</t>
         </is>
@@ -92587,7 +92587,7 @@
           <t>930</t>
         </is>
       </c>
-      <c r="J507" s="17" t="inlineStr">
+      <c r="J507" s="7" t="inlineStr">
         <is>
           <t>607</t>
         </is>
@@ -92972,7 +92972,7 @@
           <t>498</t>
         </is>
       </c>
-      <c r="E512" s="6" t="inlineStr">
+      <c r="E512" s="17" t="inlineStr">
         <is>
           <t>241</t>
         </is>
@@ -93638,7 +93638,7 @@
           <t>863</t>
         </is>
       </c>
-      <c r="G520" s="17" t="inlineStr">
+      <c r="G520" s="6" t="inlineStr">
         <is>
           <t>706</t>
         </is>
@@ -94011,7 +94011,7 @@
           <t>990</t>
         </is>
       </c>
-      <c r="P524" s="9" t="inlineStr">
+      <c r="P524" s="17" t="inlineStr">
         <is>
           <t>142</t>
         </is>
@@ -94175,7 +94175,7 @@
           <t>058</t>
         </is>
       </c>
-      <c r="P526" s="17" t="inlineStr">
+      <c r="P526" s="9" t="inlineStr">
         <is>
           <t>067</t>
         </is>
@@ -94222,7 +94222,7 @@
           <t>797</t>
         </is>
       </c>
-      <c r="I527" s="7" t="inlineStr">
+      <c r="I527" s="17" t="inlineStr">
         <is>
           <t>412</t>
         </is>

</xml_diff>

<commit_message>
move unused scripts; script_gap_common_pair.py looks promising
</commit_message>
<xml_diff>
--- a/swertres/excel_results_4.xlsx
+++ b/swertres/excel_results_4.xlsx
@@ -26,9 +26,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b val="1"/>
       <sz val="21"/>
     </font>
     <font>
+      <b val="1"/>
       <color rgb="00000000"/>
       <sz val="21"/>
     </font>
@@ -73177,7 +73179,7 @@
       </c>
       <c r="S395" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>970</t>
         </is>
       </c>
       <c r="T395" s="11" t="inlineStr">
@@ -91712,6 +91714,13 @@
       </c>
       <c r="O496" s="2" t="n"/>
       <c r="P496" s="3" t="n"/>
+      <c r="Q496" s="1" t="inlineStr">
+        <is>
+          <t>JUN 2021</t>
+        </is>
+      </c>
+      <c r="R496" s="2" t="n"/>
+      <c r="S496" s="3" t="n"/>
     </row>
     <row r="497">
       <c r="A497" s="4" t="n"/>
@@ -91790,6 +91799,21 @@
           <t>9PM</t>
         </is>
       </c>
+      <c r="Q497" s="1" t="inlineStr">
+        <is>
+          <t>2PM</t>
+        </is>
+      </c>
+      <c r="R497" s="1" t="inlineStr">
+        <is>
+          <t>4PM</t>
+        </is>
+      </c>
+      <c r="S497" s="1" t="inlineStr">
+        <is>
+          <t>9PM</t>
+        </is>
+      </c>
     </row>
     <row r="498">
       <c r="A498" s="1" t="inlineStr">
@@ -91872,6 +91896,21 @@
           <t>403</t>
         </is>
       </c>
+      <c r="Q498" s="10" t="inlineStr">
+        <is>
+          <t>362</t>
+        </is>
+      </c>
+      <c r="R498" s="10" t="inlineStr">
+        <is>
+          <t>011</t>
+        </is>
+      </c>
+      <c r="S498" s="10" t="inlineStr">
+        <is>
+          <t>778</t>
+        </is>
+      </c>
     </row>
     <row r="499">
       <c r="A499" s="1" t="inlineStr">
@@ -91954,6 +91993,21 @@
           <t>052</t>
         </is>
       </c>
+      <c r="Q499" s="10" t="inlineStr">
+        <is>
+          <t>712</t>
+        </is>
+      </c>
+      <c r="R499" s="10" t="inlineStr">
+        <is>
+          <t>985</t>
+        </is>
+      </c>
+      <c r="S499" s="10" t="inlineStr">
+        <is>
+          <t>425</t>
+        </is>
+      </c>
     </row>
     <row r="500">
       <c r="A500" s="1" t="inlineStr">
@@ -92036,6 +92090,21 @@
           <t>259</t>
         </is>
       </c>
+      <c r="Q500" s="10" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="R500" s="10" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
+      </c>
+      <c r="S500" s="10" t="inlineStr">
+        <is>
+          <t>840</t>
+        </is>
+      </c>
     </row>
     <row r="501">
       <c r="A501" s="1" t="inlineStr">
@@ -92118,6 +92187,21 @@
           <t>308</t>
         </is>
       </c>
+      <c r="Q501" s="10" t="inlineStr">
+        <is>
+          <t>883</t>
+        </is>
+      </c>
+      <c r="R501" s="10" t="inlineStr">
+        <is>
+          <t>199</t>
+        </is>
+      </c>
+      <c r="S501" s="10" t="inlineStr">
+        <is>
+          <t>845</t>
+        </is>
+      </c>
     </row>
     <row r="502">
       <c r="A502" s="1" t="inlineStr">
@@ -92200,6 +92284,21 @@
           <t>789</t>
         </is>
       </c>
+      <c r="Q502" s="10" t="inlineStr">
+        <is>
+          <t>992</t>
+        </is>
+      </c>
+      <c r="R502" s="10" t="inlineStr">
+        <is>
+          <t>346</t>
+        </is>
+      </c>
+      <c r="S502" s="10" t="inlineStr">
+        <is>
+          <t>055</t>
+        </is>
+      </c>
     </row>
     <row r="503">
       <c r="A503" s="1" t="inlineStr">
@@ -92282,6 +92381,21 @@
           <t>417</t>
         </is>
       </c>
+      <c r="Q503" s="10" t="inlineStr">
+        <is>
+          <t>793</t>
+        </is>
+      </c>
+      <c r="R503" s="10" t="inlineStr">
+        <is>
+          <t>816</t>
+        </is>
+      </c>
+      <c r="S503" s="10" t="inlineStr">
+        <is>
+          <t>637</t>
+        </is>
+      </c>
     </row>
     <row r="504">
       <c r="A504" s="1" t="inlineStr">
@@ -92364,6 +92478,21 @@
           <t>635</t>
         </is>
       </c>
+      <c r="Q504" s="10" t="inlineStr">
+        <is>
+          <t>231</t>
+        </is>
+      </c>
+      <c r="R504" s="10" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="S504" s="10" t="inlineStr">
+        <is>
+          <t>754</t>
+        </is>
+      </c>
     </row>
     <row r="505">
       <c r="A505" s="1" t="inlineStr">
@@ -92446,6 +92575,21 @@
           <t>148</t>
         </is>
       </c>
+      <c r="Q505" s="10" t="inlineStr">
+        <is>
+          <t>794</t>
+        </is>
+      </c>
+      <c r="R505" s="10" t="inlineStr">
+        <is>
+          <t>249</t>
+        </is>
+      </c>
+      <c r="S505" s="10" t="inlineStr">
+        <is>
+          <t>430</t>
+        </is>
+      </c>
     </row>
     <row r="506">
       <c r="A506" s="1" t="inlineStr">
@@ -92528,6 +92672,21 @@
           <t>380</t>
         </is>
       </c>
+      <c r="Q506" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R506" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S506" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="507">
       <c r="A507" s="1" t="inlineStr">
@@ -92610,6 +92769,21 @@
           <t>373</t>
         </is>
       </c>
+      <c r="Q507" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R507" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S507" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="508">
       <c r="A508" s="1" t="inlineStr">
@@ -92692,6 +92866,21 @@
           <t>536</t>
         </is>
       </c>
+      <c r="Q508" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R508" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S508" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="509">
       <c r="A509" s="1" t="inlineStr">
@@ -92774,6 +92963,21 @@
           <t>881</t>
         </is>
       </c>
+      <c r="Q509" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R509" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S509" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="510">
       <c r="A510" s="1" t="inlineStr">
@@ -92856,6 +93060,21 @@
           <t>236</t>
         </is>
       </c>
+      <c r="Q510" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R510" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S510" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="511">
       <c r="A511" s="1" t="inlineStr">
@@ -92938,6 +93157,21 @@
           <t>066</t>
         </is>
       </c>
+      <c r="Q511" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R511" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S511" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="512">
       <c r="A512" s="1" t="inlineStr">
@@ -93020,6 +93254,21 @@
           <t>637</t>
         </is>
       </c>
+      <c r="Q512" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R512" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S512" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="513">
       <c r="A513" s="1" t="inlineStr">
@@ -93102,6 +93351,21 @@
           <t>116</t>
         </is>
       </c>
+      <c r="Q513" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R513" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S513" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="514">
       <c r="A514" s="1" t="inlineStr">
@@ -93184,6 +93448,21 @@
           <t>244</t>
         </is>
       </c>
+      <c r="Q514" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R514" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S514" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="515">
       <c r="A515" s="1" t="inlineStr">
@@ -93266,6 +93545,21 @@
           <t>374</t>
         </is>
       </c>
+      <c r="Q515" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R515" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S515" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="516">
       <c r="A516" s="1" t="inlineStr">
@@ -93348,6 +93642,21 @@
           <t>592</t>
         </is>
       </c>
+      <c r="Q516" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R516" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S516" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="517">
       <c r="A517" s="1" t="inlineStr">
@@ -93430,6 +93739,21 @@
           <t>564</t>
         </is>
       </c>
+      <c r="Q517" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R517" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S517" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="518">
       <c r="A518" s="1" t="inlineStr">
@@ -93512,6 +93836,21 @@
           <t>209</t>
         </is>
       </c>
+      <c r="Q518" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R518" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S518" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="519">
       <c r="A519" s="1" t="inlineStr">
@@ -93594,6 +93933,21 @@
           <t>054</t>
         </is>
       </c>
+      <c r="Q519" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R519" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S519" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="520">
       <c r="A520" s="1" t="inlineStr">
@@ -93676,6 +94030,21 @@
           <t>179</t>
         </is>
       </c>
+      <c r="Q520" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R520" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S520" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="521">
       <c r="A521" s="1" t="inlineStr">
@@ -93758,6 +94127,21 @@
           <t>153</t>
         </is>
       </c>
+      <c r="Q521" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R521" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S521" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="522">
       <c r="A522" s="1" t="inlineStr">
@@ -93840,6 +94224,21 @@
           <t>198</t>
         </is>
       </c>
+      <c r="Q522" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R522" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S522" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="523">
       <c r="A523" s="1" t="inlineStr">
@@ -93922,6 +94321,21 @@
           <t>714</t>
         </is>
       </c>
+      <c r="Q523" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R523" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S523" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="524">
       <c r="A524" s="1" t="inlineStr">
@@ -94004,6 +94418,21 @@
           <t>142</t>
         </is>
       </c>
+      <c r="Q524" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R524" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S524" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="525">
       <c r="A525" s="1" t="inlineStr">
@@ -94086,6 +94515,21 @@
           <t>305</t>
         </is>
       </c>
+      <c r="Q525" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R525" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S525" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="526">
       <c r="A526" s="1" t="inlineStr">
@@ -94168,6 +94612,21 @@
           <t>067</t>
         </is>
       </c>
+      <c r="Q526" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R526" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S526" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="527">
       <c r="A527" s="1" t="inlineStr">
@@ -94250,6 +94709,21 @@
           <t>325</t>
         </is>
       </c>
+      <c r="Q527" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R527" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S527" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="528">
       <c r="A528" s="1" t="inlineStr">
@@ -94319,22 +94793,37 @@
       </c>
       <c r="N528" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>513</t>
         </is>
       </c>
       <c r="O528" s="9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>286</t>
         </is>
       </c>
       <c r="P528" s="9" t="inlineStr">
+        <is>
+          <t>588</t>
+        </is>
+      </c>
+      <c r="Q528" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R528" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S528" s="10" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="201">
+  <mergeCells count="202">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -94536,6 +95025,7 @@
     <mergeCell ref="H496:J496"/>
     <mergeCell ref="K496:M496"/>
     <mergeCell ref="N496:P496"/>
+    <mergeCell ref="Q496:S496"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
increase gap limit to 51; move unused scripts and screenshots
</commit_message>
<xml_diff>
--- a/swertres/excel_results_4.xlsx
+++ b/swertres/excel_results_4.xlsx
@@ -92674,17 +92674,17 @@
       </c>
       <c r="Q506" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>143</t>
         </is>
       </c>
       <c r="R506" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>903</t>
         </is>
       </c>
       <c r="S506" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>868</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix gap common pair v3 to process all pairs
</commit_message>
<xml_diff>
--- a/swertres/excel_results_4.xlsx
+++ b/swertres/excel_results_4.xlsx
@@ -93450,17 +93450,17 @@
       </c>
       <c r="Q514" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>211</t>
         </is>
       </c>
       <c r="R514" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>082</t>
         </is>
       </c>
       <c r="S514" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>750</t>
         </is>
       </c>
     </row>
@@ -93547,17 +93547,17 @@
       </c>
       <c r="Q515" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>617</t>
         </is>
       </c>
       <c r="R515" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>800</t>
         </is>
       </c>
       <c r="S515" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>776</t>
         </is>
       </c>
     </row>
@@ -93644,17 +93644,17 @@
       </c>
       <c r="Q516" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>324</t>
         </is>
       </c>
       <c r="R516" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>381</t>
         </is>
       </c>
       <c r="S516" s="10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>108</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update results, confirmed gap_v3
</commit_message>
<xml_diff>
--- a/swertres/excel_results_4.xlsx
+++ b/swertres/excel_results_4.xlsx
@@ -35,7 +35,7 @@
       <sz val="21"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill/>
     </fill>
@@ -70,11 +70,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="009966ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -134,7 +129,6 @@
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,7 +208,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,11 +216,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,6 +240,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,20 +261,81 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
     <cellStyle name="def_style" xfId="1" hidden="0"/>
     <cellStyle name="res_style" xfId="2" hidden="0"/>
-    <cellStyle name="res_macth_style" xfId="3" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1920,7 +1975,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S8" s="17" t="inlineStr">
+      <c r="S8" s="10" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -3775,7 +3830,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P18" s="17" t="inlineStr">
+      <c r="P18" s="9" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -5740,7 +5795,7 @@
           <t>616</t>
         </is>
       </c>
-      <c r="AI28" s="17" t="inlineStr">
+      <c r="AI28" s="16" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -6124,7 +6179,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AK30" s="17" t="inlineStr">
+      <c r="AK30" s="16" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -6438,7 +6493,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Y32" s="17" t="inlineStr">
+      <c r="Y32" s="12" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -8208,7 +8263,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Y42" s="17" t="inlineStr">
+      <c r="Y42" s="12" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -8841,7 +8896,7 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B46" s="17" t="inlineStr">
+      <c r="B46" s="5" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -9537,7 +9592,7 @@
           <t>260</t>
         </is>
       </c>
-      <c r="AC49" s="17" t="inlineStr">
+      <c r="AC49" s="14" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -10669,7 +10724,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AE55" s="17" t="inlineStr">
+      <c r="AE55" s="14" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -10928,7 +10983,7 @@
           <t>185</t>
         </is>
       </c>
-      <c r="H57" s="17" t="inlineStr">
+      <c r="H57" s="7" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -13202,7 +13257,7 @@
           <t>626</t>
         </is>
       </c>
-      <c r="AH69" s="17" t="inlineStr">
+      <c r="AH69" s="15" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -14805,7 +14860,7 @@
           <t>061</t>
         </is>
       </c>
-      <c r="R78" s="17" t="inlineStr">
+      <c r="R78" s="10" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -15229,7 +15284,7 @@
           <t>801</t>
         </is>
       </c>
-      <c r="AB80" s="17" t="inlineStr">
+      <c r="AB80" s="13" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -15386,7 +15441,7 @@
           <t>349</t>
         </is>
       </c>
-      <c r="V81" s="17" t="inlineStr">
+      <c r="V81" s="11" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -15401,7 +15456,7 @@
           <t>933</t>
         </is>
       </c>
-      <c r="Y81" s="17" t="inlineStr">
+      <c r="Y81" s="12" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -15518,7 +15573,7 @@
           <t>559</t>
         </is>
       </c>
-      <c r="K82" s="17" t="inlineStr">
+      <c r="K82" s="8" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -16261,7 +16316,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J86" s="17" t="inlineStr">
+      <c r="J86" s="7" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -16887,7 +16942,7 @@
           <t>889</t>
         </is>
       </c>
-      <c r="W89" s="17" t="inlineStr">
+      <c r="W89" s="12" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -17463,7 +17518,7 @@
           <t>254</t>
         </is>
       </c>
-      <c r="Z92" s="17" t="inlineStr">
+      <c r="Z92" s="13" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -17877,7 +17932,7 @@
           <t>679</t>
         </is>
       </c>
-      <c r="AH94" s="17" t="inlineStr">
+      <c r="AH94" s="15" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -17939,7 +17994,7 @@
           <t>922</t>
         </is>
       </c>
-      <c r="I95" s="17" t="inlineStr">
+      <c r="I95" s="7" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -19809,7 +19864,7 @@
           <t>784</t>
         </is>
       </c>
-      <c r="AC105" s="17" t="inlineStr">
+      <c r="AC105" s="14" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -20532,7 +20587,7 @@
           <t>781</t>
         </is>
       </c>
-      <c r="X109" s="17" t="inlineStr">
+      <c r="X109" s="12" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -20801,7 +20856,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="C111" s="17" t="inlineStr">
+      <c r="C111" s="5" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -21230,7 +21285,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N113" s="17" t="inlineStr">
+      <c r="N113" s="9" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -21629,7 +21684,7 @@
           <t>752</t>
         </is>
       </c>
-      <c r="S115" s="17" t="inlineStr">
+      <c r="S115" s="10" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -21679,7 +21734,7 @@
           <t>112</t>
         </is>
       </c>
-      <c r="AC115" s="17" t="inlineStr">
+      <c r="AC115" s="14" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -21821,7 +21876,7 @@
           <t>080</t>
         </is>
       </c>
-      <c r="T116" s="17" t="inlineStr">
+      <c r="T116" s="11" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -22155,7 +22210,7 @@
           <t>074</t>
         </is>
       </c>
-      <c r="L118" s="17" t="inlineStr">
+      <c r="L118" s="8" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -22185,7 +22240,7 @@
           <t>129</t>
         </is>
       </c>
-      <c r="R118" s="17" t="inlineStr">
+      <c r="R118" s="10" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -22938,7 +22993,7 @@
           <t>532</t>
         </is>
       </c>
-      <c r="S122" s="17" t="inlineStr">
+      <c r="S122" s="10" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -23060,7 +23115,7 @@
           <t>808</t>
         </is>
       </c>
-      <c r="F123" s="17" t="inlineStr">
+      <c r="F123" s="6" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -23788,7 +23843,7 @@
           <t>26</t>
         </is>
       </c>
-      <c r="B127" s="17" t="inlineStr">
+      <c r="B127" s="5" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -24354,7 +24409,7 @@
           <t>793</t>
         </is>
       </c>
-      <c r="C130" s="17" t="inlineStr">
+      <c r="C130" s="5" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -24409,7 +24464,7 @@
           <t>876</t>
         </is>
       </c>
-      <c r="N130" s="17" t="inlineStr">
+      <c r="N130" s="9" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -24586,7 +24641,7 @@
           <t>245</t>
         </is>
       </c>
-      <c r="L131" s="17" t="inlineStr">
+      <c r="L131" s="8" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -24733,7 +24788,7 @@
           <t>511</t>
         </is>
       </c>
-      <c r="D132" s="17" t="inlineStr">
+      <c r="D132" s="5" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -25329,7 +25384,7 @@
           <t>992</t>
         </is>
       </c>
-      <c r="AE135" s="17" t="inlineStr">
+      <c r="AE135" s="14" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -25775,7 +25830,7 @@
           <t>129</t>
         </is>
       </c>
-      <c r="H138" s="17" t="inlineStr">
+      <c r="H138" s="7" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -25815,7 +25870,7 @@
           <t>004</t>
         </is>
       </c>
-      <c r="P138" s="17" t="inlineStr">
+      <c r="P138" s="9" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -27124,7 +27179,7 @@
           <t>298</t>
         </is>
       </c>
-      <c r="P145" s="17" t="inlineStr">
+      <c r="P145" s="9" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -27518,7 +27573,7 @@
           <t>340</t>
         </is>
       </c>
-      <c r="T147" s="17" t="inlineStr">
+      <c r="T147" s="11" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -27573,7 +27628,7 @@
           <t>808</t>
         </is>
       </c>
-      <c r="AE147" s="17" t="inlineStr">
+      <c r="AE147" s="14" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -28241,7 +28296,7 @@
           <t>146</t>
         </is>
       </c>
-      <c r="O151" s="17" t="inlineStr">
+      <c r="O151" s="9" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -28610,7 +28665,7 @@
           <t>551</t>
         </is>
       </c>
-      <c r="N153" s="17" t="inlineStr">
+      <c r="N153" s="9" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -28655,7 +28710,7 @@
           <t>872</t>
         </is>
       </c>
-      <c r="W153" s="17" t="inlineStr">
+      <c r="W153" s="12" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -29343,7 +29398,7 @@
           <t>322</t>
         </is>
       </c>
-      <c r="K157" s="17" t="inlineStr">
+      <c r="K157" s="8" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -29682,7 +29737,7 @@
           <t>846</t>
         </is>
       </c>
-      <c r="D159" s="17" t="inlineStr">
+      <c r="D159" s="5" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -29994,7 +30049,7 @@
           <t>399</t>
         </is>
       </c>
-      <c r="AC160" s="17" t="inlineStr">
+      <c r="AC160" s="14" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -31552,7 +31607,7 @@
           <t>592</t>
         </is>
       </c>
-      <c r="X169" s="17" t="inlineStr">
+      <c r="X169" s="12" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -31831,7 +31886,7 @@
           <t>452</t>
         </is>
       </c>
-      <c r="E171" s="17" t="inlineStr">
+      <c r="E171" s="6" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -32674,7 +32729,7 @@
           <t>938</t>
         </is>
       </c>
-      <c r="X175" s="17" t="inlineStr">
+      <c r="X175" s="12" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -33108,7 +33163,7 @@
           <t>038</t>
         </is>
       </c>
-      <c r="AJ177" s="17" t="inlineStr">
+      <c r="AJ177" s="16" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -33407,7 +33462,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="U179" s="17" t="inlineStr">
+      <c r="U179" s="11" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -33649,7 +33704,7 @@
           <t>661</t>
         </is>
       </c>
-      <c r="AF180" s="17" t="inlineStr">
+      <c r="AF180" s="15" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -34150,7 +34205,7 @@
           <t>706</t>
         </is>
       </c>
-      <c r="T183" s="17" t="inlineStr">
+      <c r="T183" s="11" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -34367,7 +34422,7 @@
           <t>292</t>
         </is>
       </c>
-      <c r="Z184" s="17" t="inlineStr">
+      <c r="Z184" s="13" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -34449,7 +34504,7 @@
           <t>674</t>
         </is>
       </c>
-      <c r="E185" s="17" t="inlineStr">
+      <c r="E185" s="6" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -36127,7 +36182,7 @@
           <t>223</t>
         </is>
       </c>
-      <c r="D194" s="17" t="inlineStr">
+      <c r="D194" s="5" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -37030,7 +37085,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="AI198" s="17" t="inlineStr">
+      <c r="AI198" s="16" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -37790,7 +37845,7 @@
           <t>164</t>
         </is>
       </c>
-      <c r="T203" s="17" t="inlineStr">
+      <c r="T203" s="11" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -38139,7 +38194,7 @@
           <t>825</t>
         </is>
       </c>
-      <c r="O205" s="17" t="inlineStr">
+      <c r="O205" s="9" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -38386,7 +38441,7 @@
           <t>979</t>
         </is>
       </c>
-      <c r="AA206" s="17" t="inlineStr">
+      <c r="AA206" s="13" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -38406,7 +38461,7 @@
           <t>903</t>
         </is>
       </c>
-      <c r="AE206" s="17" t="inlineStr">
+      <c r="AE206" s="14" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -39610,7 +39665,7 @@
           <t>554</t>
         </is>
       </c>
-      <c r="J213" s="17" t="inlineStr">
+      <c r="J213" s="7" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -39665,7 +39720,7 @@
           <t>444</t>
         </is>
       </c>
-      <c r="U213" s="17" t="inlineStr">
+      <c r="U213" s="11" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -40109,7 +40164,7 @@
           <t>037</t>
         </is>
       </c>
-      <c r="AI215" s="17" t="inlineStr">
+      <c r="AI215" s="16" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -40767,7 +40822,7 @@
           <t>798</t>
         </is>
       </c>
-      <c r="Q219" s="17" t="inlineStr">
+      <c r="Q219" s="10" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -41081,7 +41136,7 @@
           <t>783</t>
         </is>
       </c>
-      <c r="E221" s="17" t="inlineStr">
+      <c r="E221" s="6" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -41313,7 +41368,7 @@
           <t>413</t>
         </is>
       </c>
-      <c r="N222" s="17" t="inlineStr">
+      <c r="N222" s="9" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -42066,7 +42121,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="O226" s="17" t="inlineStr">
+      <c r="O226" s="9" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -42617,7 +42672,7 @@
           <t>623</t>
         </is>
       </c>
-      <c r="M229" s="17" t="inlineStr">
+      <c r="M229" s="8" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -43634,7 +43689,7 @@
           <t>657</t>
         </is>
       </c>
-      <c r="L235" s="17" t="inlineStr">
+      <c r="L235" s="8" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -44654,7 +44709,7 @@
           <t>541</t>
         </is>
       </c>
-      <c r="AC240" s="17" t="inlineStr">
+      <c r="AC240" s="14" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -44731,7 +44786,7 @@
           <t>527</t>
         </is>
       </c>
-      <c r="G241" s="17" t="inlineStr">
+      <c r="G241" s="6" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -45165,7 +45220,7 @@
           <t>148</t>
         </is>
       </c>
-      <c r="S243" s="17" t="inlineStr">
+      <c r="S243" s="10" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -45245,7 +45300,7 @@
           <t>691</t>
         </is>
       </c>
-      <c r="AI243" s="17" t="inlineStr">
+      <c r="AI243" s="16" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -45317,7 +45372,7 @@
           <t>088</t>
         </is>
       </c>
-      <c r="L244" s="17" t="inlineStr">
+      <c r="L244" s="8" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -45766,7 +45821,7 @@
           <t>940</t>
         </is>
       </c>
-      <c r="AA246" s="17" t="inlineStr">
+      <c r="AA246" s="13" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -45968,7 +46023,7 @@
           <t>131</t>
         </is>
       </c>
-      <c r="AD247" s="17" t="inlineStr">
+      <c r="AD247" s="14" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -46237,7 +46292,7 @@
           <t>336</t>
         </is>
       </c>
-      <c r="I249" s="17" t="inlineStr">
+      <c r="I249" s="7" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -47297,7 +47352,7 @@
           <t>372</t>
         </is>
       </c>
-      <c r="AH254" s="17" t="inlineStr">
+      <c r="AH254" s="15" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -47409,7 +47464,7 @@
           <t>367</t>
         </is>
       </c>
-      <c r="S255" s="17" t="inlineStr">
+      <c r="S255" s="10" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -47863,7 +47918,7 @@
           <t>068</t>
         </is>
       </c>
-      <c r="AI257" s="17" t="inlineStr">
+      <c r="AI257" s="16" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -47873,7 +47928,7 @@
           <t>062</t>
         </is>
       </c>
-      <c r="AK257" s="17" t="inlineStr">
+      <c r="AK257" s="16" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -48132,7 +48187,7 @@
           <t>359</t>
         </is>
       </c>
-      <c r="N259" s="17" t="inlineStr">
+      <c r="N259" s="9" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -48289,7 +48344,7 @@
           <t>337</t>
         </is>
       </c>
-      <c r="H260" s="17" t="inlineStr">
+      <c r="H260" s="7" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -48304,7 +48359,7 @@
           <t>653</t>
         </is>
       </c>
-      <c r="K260" s="17" t="inlineStr">
+      <c r="K260" s="8" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -48374,7 +48429,7 @@
           <t>026</t>
         </is>
       </c>
-      <c r="Y260" s="17" t="inlineStr">
+      <c r="Y260" s="12" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -48546,7 +48601,7 @@
           <t>989</t>
         </is>
       </c>
-      <c r="V261" s="17" t="inlineStr">
+      <c r="V261" s="11" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -50221,7 +50276,7 @@
           <t>886</t>
         </is>
       </c>
-      <c r="C271" s="17" t="inlineStr">
+      <c r="C271" s="5" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -50478,7 +50533,7 @@
           <t>303</t>
         </is>
       </c>
-      <c r="Q272" s="17" t="inlineStr">
+      <c r="Q272" s="10" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -50685,7 +50740,7 @@
           <t>511</t>
         </is>
       </c>
-      <c r="U273" s="17" t="inlineStr">
+      <c r="U273" s="11" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -50892,7 +50947,7 @@
           <t>610</t>
         </is>
       </c>
-      <c r="Y274" s="17" t="inlineStr">
+      <c r="Y274" s="12" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -51241,7 +51296,7 @@
           <t>638</t>
         </is>
       </c>
-      <c r="T276" s="17" t="inlineStr">
+      <c r="T276" s="11" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -51443,7 +51498,7 @@
           <t>793</t>
         </is>
       </c>
-      <c r="W277" s="17" t="inlineStr">
+      <c r="W277" s="12" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -51620,7 +51675,7 @@
           <t>868</t>
         </is>
       </c>
-      <c r="U278" s="17" t="inlineStr">
+      <c r="U278" s="11" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -52470,7 +52525,7 @@
           <t>079</t>
         </is>
       </c>
-      <c r="D283" s="17" t="inlineStr">
+      <c r="D283" s="5" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -52802,7 +52857,7 @@
           <t>595</t>
         </is>
       </c>
-      <c r="AG284" s="17" t="inlineStr">
+      <c r="AG284" s="15" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -52964,7 +53019,7 @@
           <t>143</t>
         </is>
       </c>
-      <c r="AB285" s="17" t="inlineStr">
+      <c r="AB285" s="13" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -53859,7 +53914,7 @@
           <t>480</t>
         </is>
       </c>
-      <c r="T290" s="17" t="inlineStr">
+      <c r="T290" s="11" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -54071,7 +54126,7 @@
           <t>759</t>
         </is>
       </c>
-      <c r="Y291" s="17" t="inlineStr">
+      <c r="Y291" s="12" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -56265,7 +56320,7 @@
           <t>511</t>
         </is>
       </c>
-      <c r="AI303" s="17" t="inlineStr">
+      <c r="AI303" s="16" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -57070,7 +57125,7 @@
           <t>823</t>
         </is>
       </c>
-      <c r="I308" s="17" t="inlineStr">
+      <c r="I308" s="7" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -57160,7 +57215,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="AA308" s="17" t="inlineStr">
+      <c r="AA308" s="13" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -57726,7 +57781,7 @@
           <t>134</t>
         </is>
       </c>
-      <c r="AB311" s="17" t="inlineStr">
+      <c r="AB311" s="13" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -57741,7 +57796,7 @@
           <t>321</t>
         </is>
       </c>
-      <c r="AE311" s="17" t="inlineStr">
+      <c r="AE311" s="14" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -58110,7 +58165,7 @@
           <t>960</t>
         </is>
       </c>
-      <c r="AD313" s="17" t="inlineStr">
+      <c r="AD313" s="14" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -58394,7 +58449,7 @@
           <t>952</t>
         </is>
       </c>
-      <c r="L315" s="17" t="inlineStr">
+      <c r="L315" s="8" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -58489,7 +58544,7 @@
           <t>786</t>
         </is>
       </c>
-      <c r="AE315" s="17" t="inlineStr">
+      <c r="AE315" s="14" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -58631,7 +58686,7 @@
           <t>533</t>
         </is>
       </c>
-      <c r="V316" s="17" t="inlineStr">
+      <c r="V316" s="11" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -58955,7 +59010,7 @@
           <t>727</t>
         </is>
       </c>
-      <c r="L318" s="17" t="inlineStr">
+      <c r="L318" s="8" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -60102,7 +60157,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="Q324" s="17" t="inlineStr">
+      <c r="Q324" s="10" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -60673,7 +60728,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="S327" s="17" t="inlineStr">
+      <c r="S327" s="10" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -61999,7 +62054,7 @@
           <t>271</t>
         </is>
       </c>
-      <c r="E335" s="17" t="inlineStr">
+      <c r="E335" s="6" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -62478,7 +62533,7 @@
           <t>146</t>
         </is>
       </c>
-      <c r="Z337" s="17" t="inlineStr">
+      <c r="Z337" s="13" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -62924,7 +62979,7 @@
           <t>914</t>
         </is>
       </c>
-      <c r="C340" s="17" t="inlineStr">
+      <c r="C340" s="5" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -63211,7 +63266,7 @@
           <t>553</t>
         </is>
       </c>
-      <c r="W341" s="17" t="inlineStr">
+      <c r="W341" s="12" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -63393,7 +63448,7 @@
           <t>871</t>
         </is>
       </c>
-      <c r="V342" s="17" t="inlineStr">
+      <c r="V342" s="11" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -63463,7 +63518,7 @@
           <t>746</t>
         </is>
       </c>
-      <c r="AJ342" s="17" t="inlineStr">
+      <c r="AJ342" s="16" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -63540,7 +63595,7 @@
           <t>191</t>
         </is>
       </c>
-      <c r="N343" s="17" t="inlineStr">
+      <c r="N343" s="9" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -63782,7 +63837,7 @@
           <t>735</t>
         </is>
       </c>
-      <c r="Y344" s="17" t="inlineStr">
+      <c r="Y344" s="12" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -64602,7 +64657,7 @@
           <t>17</t>
         </is>
       </c>
-      <c r="B349" s="17" t="inlineStr">
+      <c r="B349" s="5" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -64632,7 +64687,7 @@
           <t>795</t>
         </is>
       </c>
-      <c r="H349" s="17" t="inlineStr">
+      <c r="H349" s="7" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -65136,7 +65191,7 @@
           <t>424</t>
         </is>
       </c>
-      <c r="AH351" s="17" t="inlineStr">
+      <c r="AH351" s="15" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -65173,7 +65228,7 @@
           <t>437</t>
         </is>
       </c>
-      <c r="D352" s="17" t="inlineStr">
+      <c r="D352" s="5" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -65425,7 +65480,7 @@
           <t>906</t>
         </is>
       </c>
-      <c r="Q353" s="17" t="inlineStr">
+      <c r="Q353" s="10" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -65819,7 +65874,7 @@
           <t>659</t>
         </is>
       </c>
-      <c r="U355" s="17" t="inlineStr">
+      <c r="U355" s="11" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -65859,7 +65914,7 @@
           <t>067</t>
         </is>
       </c>
-      <c r="AC355" s="17" t="inlineStr">
+      <c r="AC355" s="14" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -66218,7 +66273,7 @@
           <t>278</t>
         </is>
       </c>
-      <c r="Z357" s="17" t="inlineStr">
+      <c r="Z357" s="13" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -66455,7 +66510,7 @@
           <t>266</t>
         </is>
       </c>
-      <c r="AJ358" s="17" t="inlineStr">
+      <c r="AJ358" s="16" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -66487,7 +66542,7 @@
           <t>587</t>
         </is>
       </c>
-      <c r="E359" s="17" t="inlineStr">
+      <c r="E359" s="6" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -66946,7 +67001,7 @@
           <t>994</t>
         </is>
       </c>
-      <c r="V361" s="17" t="inlineStr">
+      <c r="V361" s="11" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -69202,7 +69257,7 @@
           <t>387</t>
         </is>
       </c>
-      <c r="G374" s="17" t="inlineStr">
+      <c r="G374" s="6" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -69379,7 +69434,7 @@
           <t>510</t>
         </is>
       </c>
-      <c r="E375" s="17" t="inlineStr">
+      <c r="E375" s="6" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -69798,7 +69853,7 @@
           <t>169</t>
         </is>
       </c>
-      <c r="N377" s="17" t="inlineStr">
+      <c r="N377" s="9" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -69828,7 +69883,7 @@
           <t>402</t>
         </is>
       </c>
-      <c r="T377" s="17" t="inlineStr">
+      <c r="T377" s="11" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -69995,7 +70050,7 @@
           <t>347</t>
         </is>
       </c>
-      <c r="P378" s="17" t="inlineStr">
+      <c r="P378" s="9" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -70122,7 +70177,7 @@
           <t>373</t>
         </is>
       </c>
-      <c r="D379" s="17" t="inlineStr">
+      <c r="D379" s="5" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -70621,7 +70676,7 @@
           <t>604</t>
         </is>
       </c>
-      <c r="AC381" s="17" t="inlineStr">
+      <c r="AC381" s="14" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -71763,7 +71818,7 @@
           <t>495</t>
         </is>
       </c>
-      <c r="AG387" s="17" t="inlineStr">
+      <c r="AG387" s="15" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -71925,7 +71980,7 @@
           <t>748</t>
         </is>
       </c>
-      <c r="AB388" s="17" t="inlineStr">
+      <c r="AB388" s="13" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -72416,7 +72471,7 @@
           <t>744</t>
         </is>
       </c>
-      <c r="N391" s="17" t="inlineStr">
+      <c r="N391" s="9" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -72501,7 +72556,7 @@
           <t>885</t>
         </is>
       </c>
-      <c r="AE391" s="17" t="inlineStr">
+      <c r="AE391" s="14" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -72638,7 +72693,7 @@
           <t>389</t>
         </is>
       </c>
-      <c r="U392" s="17" t="inlineStr">
+      <c r="U392" s="11" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -72730,7 +72785,7 @@
           <t>28</t>
         </is>
       </c>
-      <c r="B393" s="17" t="inlineStr">
+      <c r="B393" s="5" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -74064,7 +74119,7 @@
           <t>579</t>
         </is>
       </c>
-      <c r="AA400" s="17" t="inlineStr">
+      <c r="AA400" s="13" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -74236,7 +74291,7 @@
           <t>578</t>
         </is>
       </c>
-      <c r="X401" s="17" t="inlineStr">
+      <c r="X401" s="12" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -74291,7 +74346,7 @@
           <t>953</t>
         </is>
       </c>
-      <c r="AI401" s="17" t="inlineStr">
+      <c r="AI401" s="16" t="inlineStr">
         <is>
           <t>136</t>
         </is>
@@ -74393,7 +74448,7 @@
           <t>083</t>
         </is>
       </c>
-      <c r="R402" s="17" t="inlineStr">
+      <c r="R402" s="10" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -74428,7 +74483,7 @@
           <t>248</t>
         </is>
       </c>
-      <c r="Y402" s="17" t="inlineStr">
+      <c r="Y402" s="12" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -74473,7 +74528,7 @@
           <t>063</t>
         </is>
       </c>
-      <c r="AH402" s="17" t="inlineStr">
+      <c r="AH402" s="15" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -74570,7 +74625,7 @@
           <t>825</t>
         </is>
       </c>
-      <c r="P403" s="17" t="inlineStr">
+      <c r="P403" s="9" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -74600,7 +74655,7 @@
           <t>780</t>
         </is>
       </c>
-      <c r="V403" s="17" t="inlineStr">
+      <c r="V403" s="11" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -74969,7 +75024,7 @@
           <t>253</t>
         </is>
       </c>
-      <c r="U405" s="17" t="inlineStr">
+      <c r="U405" s="11" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -75081,7 +75136,7 @@
           <t>138</t>
         </is>
       </c>
-      <c r="F406" s="17" t="inlineStr">
+      <c r="F406" s="6" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -75176,7 +75231,7 @@
           <t>974</t>
         </is>
       </c>
-      <c r="Y406" s="17" t="inlineStr">
+      <c r="Y406" s="12" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -75338,7 +75393,7 @@
           <t>155</t>
         </is>
       </c>
-      <c r="T407" s="17" t="inlineStr">
+      <c r="T407" s="11" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -75672,7 +75727,7 @@
           <t>850</t>
         </is>
       </c>
-      <c r="L409" s="17" t="inlineStr">
+      <c r="L409" s="8" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -76323,7 +76378,7 @@
           <t>844</t>
         </is>
       </c>
-      <c r="AD412" s="17" t="inlineStr">
+      <c r="AD412" s="14" t="inlineStr">
         <is>
           <t>936</t>
         </is>
@@ -76732,7 +76787,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="AK414" s="17" t="inlineStr">
+      <c r="AK414" s="16" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -77450,7 +77505,7 @@
           <t>250</t>
         </is>
       </c>
-      <c r="AE418" s="17" t="inlineStr">
+      <c r="AE418" s="14" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -77532,7 +77587,7 @@
           <t>007</t>
         </is>
       </c>
-      <c r="J419" s="17" t="inlineStr">
+      <c r="J419" s="7" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -78053,7 +78108,7 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B422" s="17" t="inlineStr">
+      <c r="B422" s="5" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -78816,7 +78871,7 @@
           <t>164</t>
         </is>
       </c>
-      <c r="E426" s="17" t="inlineStr">
+      <c r="E426" s="6" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -79073,7 +79128,7 @@
           <t>714</t>
         </is>
       </c>
-      <c r="S427" s="17" t="inlineStr">
+      <c r="S427" s="10" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -79148,7 +79203,7 @@
           <t>258</t>
         </is>
       </c>
-      <c r="AH427" s="17" t="inlineStr">
+      <c r="AH427" s="15" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -79908,7 +79963,7 @@
           <t>598</t>
         </is>
       </c>
-      <c r="S432" s="17" t="inlineStr">
+      <c r="S432" s="10" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -80050,7 +80105,7 @@
           <t>368</t>
         </is>
       </c>
-      <c r="J433" s="17" t="inlineStr">
+      <c r="J433" s="7" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -80788,7 +80843,7 @@
           <t>695</t>
         </is>
       </c>
-      <c r="H437" s="17" t="inlineStr">
+      <c r="H437" s="7" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -80960,7 +81015,7 @@
           <t>405</t>
         </is>
       </c>
-      <c r="E438" s="17" t="inlineStr">
+      <c r="E438" s="6" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -81334,7 +81389,7 @@
           <t>419</t>
         </is>
       </c>
-      <c r="E440" s="17" t="inlineStr">
+      <c r="E440" s="6" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -82566,7 +82621,7 @@
           <t>376</t>
         </is>
       </c>
-      <c r="AA446" s="17" t="inlineStr">
+      <c r="AA446" s="13" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -82576,7 +82631,7 @@
           <t>479</t>
         </is>
       </c>
-      <c r="AC446" s="17" t="inlineStr">
+      <c r="AC446" s="14" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -83152,7 +83207,7 @@
           <t>662</t>
         </is>
       </c>
-      <c r="AF449" s="17" t="inlineStr">
+      <c r="AF449" s="15" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -83673,7 +83728,7 @@
           <t>807</t>
         </is>
       </c>
-      <c r="X452" s="17" t="inlineStr">
+      <c r="X452" s="12" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -84082,7 +84137,7 @@
           <t>160</t>
         </is>
       </c>
-      <c r="AE454" s="17" t="inlineStr">
+      <c r="AE454" s="14" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -84361,7 +84416,7 @@
           <t>176</t>
         </is>
       </c>
-      <c r="L456" s="17" t="inlineStr">
+      <c r="L456" s="8" t="inlineStr">
         <is>
           <t>613</t>
         </is>
@@ -84795,7 +84850,7 @@
           <t>441</t>
         </is>
       </c>
-      <c r="X458" s="17" t="inlineStr">
+      <c r="X458" s="12" t="inlineStr">
         <is>
           <t>396</t>
         </is>
@@ -85119,7 +85174,7 @@
           <t>083</t>
         </is>
       </c>
-      <c r="N460" s="17" t="inlineStr">
+      <c r="N460" s="9" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -85608,7 +85663,7 @@
           <t>745</t>
         </is>
       </c>
-      <c r="AK462" s="17" t="inlineStr">
+      <c r="AK462" s="16" t="inlineStr">
         <is>
           <t>963</t>
         </is>
@@ -87171,7 +87226,7 @@
           <t>490</t>
         </is>
       </c>
-      <c r="AG471" s="17" t="inlineStr">
+      <c r="AG471" s="15" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -88734,7 +88789,7 @@
           <t>687</t>
         </is>
       </c>
-      <c r="I480" s="17" t="inlineStr">
+      <c r="I480" s="7" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -90584,7 +90639,7 @@
           <t>605</t>
         </is>
       </c>
-      <c r="E490" s="17" t="inlineStr">
+      <c r="E490" s="6" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -91108,7 +91163,7 @@
           <t>791</t>
         </is>
       </c>
-      <c r="AI492" s="17" t="inlineStr">
+      <c r="AI492" s="16" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -91140,7 +91195,7 @@
           <t>277</t>
         </is>
       </c>
-      <c r="D493" s="17" t="inlineStr">
+      <c r="D493" s="5" t="inlineStr">
         <is>
           <t>639</t>
         </is>
@@ -91270,7 +91325,7 @@
           <t>664</t>
         </is>
       </c>
-      <c r="AD493" s="17" t="inlineStr">
+      <c r="AD493" s="14" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -91280,7 +91335,7 @@
           <t>835</t>
         </is>
       </c>
-      <c r="AF493" s="17" t="inlineStr">
+      <c r="AF493" s="15" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -91477,7 +91532,7 @@
           <t>731</t>
         </is>
       </c>
-      <c r="AH494" s="17" t="inlineStr">
+      <c r="AH494" s="15" t="inlineStr">
         <is>
           <t>316</t>
         </is>
@@ -91740,6 +91795,13 @@
       </c>
       <c r="U496" s="2" t="n"/>
       <c r="V496" s="3" t="n"/>
+      <c r="W496" s="1" t="inlineStr">
+        <is>
+          <t>AUG 2021</t>
+        </is>
+      </c>
+      <c r="X496" s="2" t="n"/>
+      <c r="Y496" s="3" t="n"/>
     </row>
     <row r="497">
       <c r="A497" s="4" t="n"/>
@@ -91848,6 +91910,21 @@
           <t>9PM</t>
         </is>
       </c>
+      <c r="W497" s="1" t="inlineStr">
+        <is>
+          <t>2PM</t>
+        </is>
+      </c>
+      <c r="X497" s="1" t="inlineStr">
+        <is>
+          <t>4PM</t>
+        </is>
+      </c>
+      <c r="Y497" s="1" t="inlineStr">
+        <is>
+          <t>9PM</t>
+        </is>
+      </c>
     </row>
     <row r="498">
       <c r="A498" s="1" t="inlineStr">
@@ -91960,6 +92037,21 @@
           <t>648</t>
         </is>
       </c>
+      <c r="W498" s="12" t="inlineStr">
+        <is>
+          <t>116</t>
+        </is>
+      </c>
+      <c r="X498" s="12" t="inlineStr">
+        <is>
+          <t>515</t>
+        </is>
+      </c>
+      <c r="Y498" s="12" t="inlineStr">
+        <is>
+          <t>346</t>
+        </is>
+      </c>
     </row>
     <row r="499">
       <c r="A499" s="1" t="inlineStr">
@@ -92072,6 +92164,21 @@
           <t>417</t>
         </is>
       </c>
+      <c r="W499" s="12" t="inlineStr">
+        <is>
+          <t>703</t>
+        </is>
+      </c>
+      <c r="X499" s="12" t="inlineStr">
+        <is>
+          <t>378</t>
+        </is>
+      </c>
+      <c r="Y499" s="12" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
     </row>
     <row r="500">
       <c r="A500" s="1" t="inlineStr">
@@ -92184,6 +92291,21 @@
           <t>474</t>
         </is>
       </c>
+      <c r="W500" s="12" t="inlineStr">
+        <is>
+          <t>314</t>
+        </is>
+      </c>
+      <c r="X500" s="12" t="inlineStr">
+        <is>
+          <t>644</t>
+        </is>
+      </c>
+      <c r="Y500" s="12" t="inlineStr">
+        <is>
+          <t>033</t>
+        </is>
+      </c>
     </row>
     <row r="501">
       <c r="A501" s="1" t="inlineStr">
@@ -92296,6 +92418,21 @@
           <t>967</t>
         </is>
       </c>
+      <c r="W501" s="12" t="inlineStr">
+        <is>
+          <t>914</t>
+        </is>
+      </c>
+      <c r="X501" s="12" t="inlineStr">
+        <is>
+          <t>337</t>
+        </is>
+      </c>
+      <c r="Y501" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="502">
       <c r="A502" s="1" t="inlineStr">
@@ -92408,6 +92545,21 @@
           <t>572</t>
         </is>
       </c>
+      <c r="W502" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X502" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y502" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="503">
       <c r="A503" s="1" t="inlineStr">
@@ -92520,6 +92672,21 @@
           <t>807</t>
         </is>
       </c>
+      <c r="W503" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X503" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y503" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="504">
       <c r="A504" s="1" t="inlineStr">
@@ -92632,6 +92799,21 @@
           <t>491</t>
         </is>
       </c>
+      <c r="W504" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X504" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y504" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="505">
       <c r="A505" s="1" t="inlineStr">
@@ -92684,7 +92866,7 @@
           <t>681</t>
         </is>
       </c>
-      <c r="K505" s="17" t="inlineStr">
+      <c r="K505" s="8" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -92742,6 +92924,21 @@
       <c r="V505" s="11" t="inlineStr">
         <is>
           <t>285</t>
+        </is>
+      </c>
+      <c r="W505" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X505" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y505" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -92856,6 +93053,21 @@
           <t>464</t>
         </is>
       </c>
+      <c r="W506" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X506" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y506" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="507">
       <c r="A507" s="1" t="inlineStr">
@@ -92968,6 +93180,21 @@
           <t>491</t>
         </is>
       </c>
+      <c r="W507" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X507" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y507" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="508">
       <c r="A508" s="1" t="inlineStr">
@@ -93080,6 +93307,21 @@
           <t>245</t>
         </is>
       </c>
+      <c r="W508" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X508" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y508" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="509">
       <c r="A509" s="1" t="inlineStr">
@@ -93192,6 +93434,21 @@
           <t>792</t>
         </is>
       </c>
+      <c r="W509" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X509" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y509" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="510">
       <c r="A510" s="1" t="inlineStr">
@@ -93304,6 +93561,21 @@
           <t>729</t>
         </is>
       </c>
+      <c r="W510" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X510" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y510" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="511">
       <c r="A511" s="1" t="inlineStr">
@@ -93416,6 +93688,21 @@
           <t>942</t>
         </is>
       </c>
+      <c r="W511" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X511" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y511" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="512">
       <c r="A512" s="1" t="inlineStr">
@@ -93528,6 +93815,21 @@
           <t>951</t>
         </is>
       </c>
+      <c r="W512" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X512" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y512" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="513">
       <c r="A513" s="1" t="inlineStr">
@@ -93640,6 +93942,21 @@
           <t>144</t>
         </is>
       </c>
+      <c r="W513" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X513" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y513" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="514">
       <c r="A514" s="1" t="inlineStr">
@@ -93682,7 +93999,7 @@
           <t>339</t>
         </is>
       </c>
-      <c r="I514" s="17" t="inlineStr">
+      <c r="I514" s="7" t="inlineStr">
         <is>
           <t>693</t>
         </is>
@@ -93742,7 +94059,7 @@
           <t>436</t>
         </is>
       </c>
-      <c r="U514" s="17" t="inlineStr">
+      <c r="U514" s="11" t="inlineStr">
         <is>
           <t>369</t>
         </is>
@@ -93750,6 +94067,21 @@
       <c r="V514" s="11" t="inlineStr">
         <is>
           <t>211</t>
+        </is>
+      </c>
+      <c r="W514" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X514" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y514" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -93809,7 +94141,7 @@
           <t>744</t>
         </is>
       </c>
-      <c r="L515" s="17" t="inlineStr">
+      <c r="L515" s="8" t="inlineStr">
         <is>
           <t>163</t>
         </is>
@@ -93854,7 +94186,7 @@
           <t>808</t>
         </is>
       </c>
-      <c r="U515" s="17" t="inlineStr">
+      <c r="U515" s="11" t="inlineStr">
         <is>
           <t>361</t>
         </is>
@@ -93862,6 +94194,21 @@
       <c r="V515" s="11" t="inlineStr">
         <is>
           <t>949</t>
+        </is>
+      </c>
+      <c r="W515" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X515" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y515" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -93963,15 +94310,30 @@
       </c>
       <c r="T516" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>722</t>
         </is>
       </c>
       <c r="U516" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>507</t>
         </is>
       </c>
       <c r="V516" s="11" t="inlineStr">
+        <is>
+          <t>807</t>
+        </is>
+      </c>
+      <c r="W516" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X516" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y516" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94023,7 +94385,7 @@
           <t>377</t>
         </is>
       </c>
-      <c r="J517" s="17" t="inlineStr">
+      <c r="J517" s="7" t="inlineStr">
         <is>
           <t>631</t>
         </is>
@@ -94075,15 +94437,30 @@
       </c>
       <c r="T517" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>912</t>
         </is>
       </c>
       <c r="U517" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>738</t>
         </is>
       </c>
       <c r="V517" s="11" t="inlineStr">
+        <is>
+          <t>972</t>
+        </is>
+      </c>
+      <c r="W517" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X517" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y517" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94187,15 +94564,30 @@
       </c>
       <c r="T518" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>879</t>
         </is>
       </c>
       <c r="U518" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>065</t>
         </is>
       </c>
       <c r="V518" s="11" t="inlineStr">
+        <is>
+          <t>801</t>
+        </is>
+      </c>
+      <c r="W518" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X518" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y518" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94299,15 +94691,30 @@
       </c>
       <c r="T519" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>409</t>
         </is>
       </c>
       <c r="U519" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>836</t>
         </is>
       </c>
       <c r="V519" s="11" t="inlineStr">
+        <is>
+          <t>223</t>
+        </is>
+      </c>
+      <c r="W519" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X519" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y519" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94411,15 +94818,30 @@
       </c>
       <c r="T520" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>758</t>
         </is>
       </c>
       <c r="U520" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>481</t>
         </is>
       </c>
       <c r="V520" s="11" t="inlineStr">
+        <is>
+          <t>830</t>
+        </is>
+      </c>
+      <c r="W520" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X520" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y520" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94523,15 +94945,30 @@
       </c>
       <c r="T521" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>488</t>
         </is>
       </c>
       <c r="U521" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>551</t>
         </is>
       </c>
       <c r="V521" s="11" t="inlineStr">
+        <is>
+          <t>629</t>
+        </is>
+      </c>
+      <c r="W521" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X521" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y521" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94635,15 +95072,30 @@
       </c>
       <c r="T522" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>901</t>
         </is>
       </c>
       <c r="U522" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>010</t>
         </is>
       </c>
       <c r="V522" s="11" t="inlineStr">
+        <is>
+          <t>295</t>
+        </is>
+      </c>
+      <c r="W522" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X522" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y522" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94747,15 +95199,30 @@
       </c>
       <c r="T523" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>651</t>
         </is>
       </c>
       <c r="U523" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>236</t>
         </is>
       </c>
       <c r="V523" s="11" t="inlineStr">
+        <is>
+          <t>952</t>
+        </is>
+      </c>
+      <c r="W523" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X523" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y523" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94859,15 +95326,30 @@
       </c>
       <c r="T524" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>248</t>
         </is>
       </c>
       <c r="U524" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>760</t>
         </is>
       </c>
       <c r="V524" s="11" t="inlineStr">
+        <is>
+          <t>117</t>
+        </is>
+      </c>
+      <c r="W524" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X524" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y524" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -94971,15 +95453,30 @@
       </c>
       <c r="T525" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>128</t>
         </is>
       </c>
       <c r="U525" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>138</t>
         </is>
       </c>
       <c r="V525" s="11" t="inlineStr">
+        <is>
+          <t>855</t>
+        </is>
+      </c>
+      <c r="W525" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X525" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y525" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -95083,15 +95580,30 @@
       </c>
       <c r="T526" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>648</t>
         </is>
       </c>
       <c r="U526" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>797</t>
         </is>
       </c>
       <c r="V526" s="11" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="W526" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X526" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y526" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -95195,15 +95707,30 @@
       </c>
       <c r="T527" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>156</t>
         </is>
       </c>
       <c r="U527" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>057</t>
         </is>
       </c>
       <c r="V527" s="11" t="inlineStr">
+        <is>
+          <t>015</t>
+        </is>
+      </c>
+      <c r="W527" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X527" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y527" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -95307,22 +95834,37 @@
       </c>
       <c r="T528" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>433</t>
         </is>
       </c>
       <c r="U528" s="11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>721</t>
         </is>
       </c>
       <c r="V528" s="11" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="W528" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X528" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y528" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="203">
+  <mergeCells count="204">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -95526,6 +96068,7 @@
     <mergeCell ref="N496:P496"/>
     <mergeCell ref="Q496:S496"/>
     <mergeCell ref="T496:V496"/>
+    <mergeCell ref="W496:Y496"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update results; gap_pair_v3 still works
</commit_message>
<xml_diff>
--- a/swertres/excel_results_4.xlsx
+++ b/swertres/excel_results_4.xlsx
@@ -92430,7 +92430,7 @@
       </c>
       <c r="Y501" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>055</t>
         </is>
       </c>
     </row>
@@ -92547,17 +92547,17 @@
       </c>
       <c r="W502" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>131</t>
         </is>
       </c>
       <c r="X502" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>836</t>
         </is>
       </c>
       <c r="Y502" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>431</t>
         </is>
       </c>
     </row>
@@ -92674,17 +92674,17 @@
       </c>
       <c r="W503" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>068</t>
         </is>
       </c>
       <c r="X503" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>032</t>
         </is>
       </c>
       <c r="Y503" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>040</t>
         </is>
       </c>
     </row>
@@ -92801,17 +92801,17 @@
       </c>
       <c r="W504" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>418</t>
         </is>
       </c>
       <c r="X504" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>035</t>
         </is>
       </c>
       <c r="Y504" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>707</t>
         </is>
       </c>
     </row>
@@ -92928,17 +92928,17 @@
       </c>
       <c r="W505" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>438</t>
         </is>
       </c>
       <c r="X505" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>872</t>
         </is>
       </c>
       <c r="Y505" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>531</t>
         </is>
       </c>
     </row>
@@ -93055,17 +93055,17 @@
       </c>
       <c r="W506" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>950</t>
         </is>
       </c>
       <c r="X506" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>025</t>
         </is>
       </c>
       <c r="Y506" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>712</t>
         </is>
       </c>
     </row>
@@ -93182,17 +93182,17 @@
       </c>
       <c r="W507" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>240</t>
         </is>
       </c>
       <c r="X507" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>749</t>
         </is>
       </c>
       <c r="Y507" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>051</t>
         </is>
       </c>
     </row>
@@ -93309,17 +93309,17 @@
       </c>
       <c r="W508" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>862</t>
         </is>
       </c>
       <c r="X508" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>246</t>
         </is>
       </c>
       <c r="Y508" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>075</t>
         </is>
       </c>
     </row>
@@ -93436,17 +93436,17 @@
       </c>
       <c r="W509" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>194</t>
         </is>
       </c>
       <c r="X509" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>119</t>
         </is>
       </c>
       <c r="Y509" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>302</t>
         </is>
       </c>
     </row>
@@ -93563,17 +93563,17 @@
       </c>
       <c r="W510" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>294</t>
         </is>
       </c>
       <c r="X510" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>291</t>
         </is>
       </c>
       <c r="Y510" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>382</t>
         </is>
       </c>
     </row>
@@ -93690,17 +93690,17 @@
       </c>
       <c r="W511" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>531</t>
         </is>
       </c>
       <c r="X511" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>609</t>
         </is>
       </c>
       <c r="Y511" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>364</t>
         </is>
       </c>
     </row>
@@ -93817,17 +93817,17 @@
       </c>
       <c r="W512" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>021</t>
         </is>
       </c>
       <c r="X512" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>094</t>
         </is>
       </c>
       <c r="Y512" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>383</t>
         </is>
       </c>
     </row>
@@ -93944,17 +93944,17 @@
       </c>
       <c r="W513" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>879</t>
         </is>
       </c>
       <c r="X513" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>599</t>
         </is>
       </c>
       <c r="Y513" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>824</t>
         </is>
       </c>
     </row>
@@ -94071,17 +94071,17 @@
       </c>
       <c r="W514" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>606</t>
         </is>
       </c>
       <c r="X514" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>611</t>
         </is>
       </c>
       <c r="Y514" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>360</t>
         </is>
       </c>
     </row>
@@ -94198,17 +94198,17 @@
       </c>
       <c r="W515" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>696</t>
         </is>
       </c>
       <c r="X515" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>239</t>
         </is>
       </c>
       <c r="Y515" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>391</t>
         </is>
       </c>
     </row>
@@ -94325,17 +94325,17 @@
       </c>
       <c r="W516" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>636</t>
         </is>
       </c>
       <c r="X516" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>054</t>
         </is>
       </c>
       <c r="Y516" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>108</t>
         </is>
       </c>
     </row>
@@ -94452,17 +94452,17 @@
       </c>
       <c r="W517" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>386</t>
         </is>
       </c>
       <c r="X517" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>715</t>
         </is>
       </c>
       <c r="Y517" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>388</t>
         </is>
       </c>
     </row>
@@ -94579,17 +94579,17 @@
       </c>
       <c r="W518" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>612</t>
         </is>
       </c>
       <c r="X518" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>908</t>
         </is>
       </c>
       <c r="Y518" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>275</t>
         </is>
       </c>
     </row>
@@ -94706,17 +94706,17 @@
       </c>
       <c r="W519" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>633</t>
         </is>
       </c>
       <c r="X519" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>571</t>
         </is>
       </c>
       <c r="Y519" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>377</t>
         </is>
       </c>
     </row>
@@ -94833,17 +94833,17 @@
       </c>
       <c r="W520" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>608</t>
         </is>
       </c>
       <c r="X520" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>948</t>
         </is>
       </c>
       <c r="Y520" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>511</t>
         </is>
       </c>
     </row>
@@ -94960,17 +94960,17 @@
       </c>
       <c r="W521" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>496</t>
         </is>
       </c>
       <c r="X521" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>544</t>
         </is>
       </c>
       <c r="Y521" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>955</t>
         </is>
       </c>
     </row>
@@ -95087,17 +95087,17 @@
       </c>
       <c r="W522" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>484</t>
         </is>
       </c>
       <c r="X522" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>693</t>
         </is>
       </c>
       <c r="Y522" s="12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>707</t>
         </is>
       </c>
     </row>

</xml_diff>